<commit_message>
Fix difference calculations (divide by 4 - the incremental # of conditions)
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POWERPNT\Seattle UG June 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242838B8-E49F-4A2D-974A-4CD77A1BE508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615D5F2E-3C31-4983-90C8-85D622A82494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30285" yWindow="1815" windowWidth="25035" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27450" yWindow="2325" windowWidth="25035" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
   <dimension ref="A2:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,20 +903,20 @@
         <v>8</v>
       </c>
       <c r="E11">
-        <f>C10-(D10-E10)-((D10-C10)/5)</f>
-        <v>-1.9199999999999959</v>
+        <f>C10-(D10-E10)-((D10-C10)/4)</f>
+        <v>-2.1999999999999957</v>
       </c>
       <c r="H11">
-        <f>F10-(G10-H10)-((G10-F10)/5)</f>
-        <v>54.92</v>
+        <f>F10-(G10-H10)-((G10-F10)/4)</f>
+        <v>54.1</v>
       </c>
       <c r="K11">
-        <f>I10-(J10-K10)-((J10-I10)/5)</f>
-        <v>92.07999999999997</v>
+        <f>I10-(J10-K10)-((J10-I10)/4)</f>
+        <v>91.799999999999969</v>
       </c>
       <c r="N11">
-        <f>L10-(M10-N10)-((M10-L10)/5)</f>
-        <v>88.719999999999942</v>
+        <f>L10-(M10-N10)-((M10-L10)/4)</f>
+        <v>84.449999999999946</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -924,20 +924,20 @@
         <v>9</v>
       </c>
       <c r="D12">
-        <f>(D10-C10)/5</f>
-        <v>1.1199999999999988</v>
+        <f>(D10-C10)/4</f>
+        <v>1.3999999999999986</v>
       </c>
       <c r="G12">
-        <f>(G10-F10)/5</f>
-        <v>3.2800000000000011</v>
+        <f>(G10-F10)/4</f>
+        <v>4.1000000000000014</v>
       </c>
       <c r="J12">
-        <f>(J10-I10)/5</f>
-        <v>1.1200000000000045</v>
+        <f>(J10-I10)/4</f>
+        <v>1.4000000000000057</v>
       </c>
       <c r="M12">
-        <f>(M10-L10)/5</f>
-        <v>17.080000000000005</v>
+        <f>(M10-L10)/4</f>
+        <v>21.350000000000009</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>